<commit_message>
Minor fix related to tables structure
</commit_message>
<xml_diff>
--- a/Schemes/tables_structure.xlsx
+++ b/Schemes/tables_structure.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\float256\iCalendarIntegration\Schemes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>id_hotel</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>int, Not Null</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -115,10 +118,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -133,10 +136,92 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -145,100 +230,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -247,34 +248,34 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -555,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -569,84 +570,98 @@
     <col min="5" max="5" width="26.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="1"/>
       <c r="D1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="9"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E7" s="5" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>